<commit_message>
final version of autumn 2021 schedule
</commit_message>
<xml_diff>
--- a/data/elm_autumn_2021/staff_requirements.xlsx
+++ b/data/elm_autumn_2021/staff_requirements.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF11"/>
+  <dimension ref="A1:AG11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -594,6 +594,11 @@
           <t>12/11/21</t>
         </is>
       </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>11/11/21</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -756,6 +761,11 @@
           <t>-1</t>
         </is>
       </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -918,6 +928,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -1080,6 +1095,11 @@
           <t>-1</t>
         </is>
       </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>-2</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -1242,6 +1262,11 @@
           <t>-2</t>
         </is>
       </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1404,6 +1429,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1566,6 +1596,11 @@
           <t>-2</t>
         </is>
       </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1728,6 +1763,11 @@
           <t>0</t>
         </is>
       </c>
+      <c r="AG8" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1890,6 +1930,11 @@
           <t>1</t>
         </is>
       </c>
+      <c r="AG9" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -2052,6 +2097,11 @@
           <t>-1</t>
         </is>
       </c>
+      <c r="AG10" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -2210,6 +2260,11 @@
         </is>
       </c>
       <c r="AF11" t="inlineStr">
+        <is>
+          <t>-1</t>
+        </is>
+      </c>
+      <c r="AG11" t="inlineStr">
         <is>
           <t>-1</t>
         </is>

</xml_diff>